<commit_message>
Site updated: 2022-03-20 21:35:58
</commit_message>
<xml_diff>
--- a/enigma/reports/minutes_per_week 2022-03-13 12-43.xlsx
+++ b/enigma/reports/minutes_per_week 2022-03-13 12-43.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tony\Work\unified-backend\html\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF0173-21A0-4992-A37F-1B09392365E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -640,8 +646,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,6 +710,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -750,7 +764,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -782,9 +796,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -816,6 +848,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -991,14 +1041,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -1089,7 +1145,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1133,7 +1189,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1177,7 +1233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1221,7 +1277,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1265,7 +1321,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1309,7 +1365,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1323,7 +1379,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1337,7 +1393,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1381,7 +1437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-2</v>
       </c>
@@ -1425,7 +1481,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1</v>
       </c>
@@ -1469,7 +1525,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1</v>
       </c>
@@ -1513,7 +1569,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1</v>
       </c>
@@ -1557,7 +1613,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1</v>
       </c>
@@ -1601,7 +1657,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29</v>
       </c>
@@ -1645,7 +1701,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -1689,7 +1745,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
@@ -1733,7 +1789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>32</v>
       </c>
@@ -1777,7 +1833,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
@@ -1791,7 +1847,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>34</v>
       </c>
@@ -1835,7 +1891,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>35</v>
       </c>
@@ -1849,7 +1905,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>36</v>
       </c>
@@ -1863,7 +1919,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>37</v>
       </c>
@@ -1877,7 +1933,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>38</v>
       </c>
@@ -1921,7 +1977,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>39</v>
       </c>
@@ -1965,7 +2021,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>40</v>
       </c>
@@ -1979,7 +2035,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>41</v>
       </c>
@@ -2023,7 +2079,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>42</v>
       </c>
@@ -2067,7 +2123,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>43</v>
       </c>
@@ -2111,7 +2167,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>44</v>
       </c>
@@ -2155,7 +2211,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>45</v>
       </c>
@@ -2169,7 +2225,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>47</v>
       </c>
@@ -2213,7 +2269,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>48</v>
       </c>
@@ -2257,7 +2313,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50</v>
       </c>
@@ -2271,7 +2327,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>51</v>
       </c>
@@ -2285,7 +2341,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>52</v>
       </c>
@@ -2329,7 +2385,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>53</v>
       </c>
@@ -2373,7 +2429,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>55</v>
       </c>
@@ -2417,7 +2473,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>56</v>
       </c>
@@ -2431,7 +2487,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>57</v>
       </c>
@@ -2475,7 +2531,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>58</v>
       </c>
@@ -2489,7 +2545,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>59</v>
       </c>
@@ -2503,7 +2559,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>60</v>
       </c>
@@ -2547,7 +2603,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>61</v>
       </c>
@@ -2591,7 +2647,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>62</v>
       </c>
@@ -2635,7 +2691,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>63</v>
       </c>
@@ -2679,7 +2735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>64</v>
       </c>
@@ -2723,7 +2779,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>65</v>
       </c>
@@ -2767,7 +2823,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>66</v>
       </c>
@@ -2811,7 +2867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>67</v>
       </c>
@@ -2825,7 +2881,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>68</v>
       </c>
@@ -2869,7 +2925,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>69</v>
       </c>
@@ -2883,7 +2939,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-2</v>
       </c>
@@ -2927,7 +2983,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-2</v>
       </c>
@@ -2971,7 +3027,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-1</v>
       </c>
@@ -3015,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-1</v>
       </c>
@@ -3059,7 +3115,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-1</v>
       </c>
@@ -3103,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-1</v>
       </c>
@@ -3147,7 +3203,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1</v>
       </c>
@@ -3191,7 +3247,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1</v>
       </c>
@@ -3235,7 +3291,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-1</v>
       </c>
@@ -3279,7 +3335,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-1</v>
       </c>
@@ -3323,7 +3379,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-1</v>
       </c>
@@ -3367,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-1</v>
       </c>
@@ -3411,7 +3467,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-1</v>
       </c>
@@ -3455,7 +3511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-1</v>
       </c>
@@ -3499,7 +3555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-1</v>
       </c>
@@ -3543,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-1</v>
       </c>
@@ -3587,7 +3643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-1</v>
       </c>
@@ -3631,7 +3687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-1</v>
       </c>
@@ -3675,7 +3731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-1</v>
       </c>
@@ -3719,7 +3775,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-1</v>
       </c>
@@ -3763,7 +3819,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-1</v>
       </c>
@@ -3807,7 +3863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-1</v>
       </c>
@@ -3851,7 +3907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-1</v>
       </c>
@@ -3895,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-1</v>
       </c>
@@ -3939,7 +3995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-1</v>
       </c>
@@ -3983,7 +4039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-1</v>
       </c>
@@ -4027,7 +4083,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-1</v>
       </c>
@@ -4071,7 +4127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-1</v>
       </c>
@@ -4115,7 +4171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-1</v>
       </c>
@@ -4159,7 +4215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-1</v>
       </c>
@@ -4203,7 +4259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-1</v>
       </c>
@@ -4247,7 +4303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-1</v>
       </c>
@@ -4291,7 +4347,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>-1</v>
       </c>
@@ -4335,7 +4391,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>-1</v>
       </c>
@@ -4379,7 +4435,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>-1</v>
       </c>
@@ -4423,7 +4479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>-1</v>
       </c>
@@ -4467,7 +4523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>-1</v>
       </c>
@@ -4511,7 +4567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>-1</v>
       </c>
@@ -4555,7 +4611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>-1</v>
       </c>
@@ -4599,7 +4655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>-1</v>
       </c>
@@ -4643,7 +4699,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>-1</v>
       </c>
@@ -4687,7 +4743,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>-1</v>
       </c>
@@ -4731,7 +4787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>-1</v>
       </c>
@@ -4775,7 +4831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>-1</v>
       </c>
@@ -4819,7 +4875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>-1</v>
       </c>
@@ -4863,7 +4919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>-1</v>
       </c>
@@ -4907,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>-1</v>
       </c>
@@ -4951,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>-1</v>
       </c>
@@ -4995,7 +5051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>-1</v>
       </c>

</xml_diff>